<commit_message>
Durchmesser zu excel Kantenverteilung/GESAMT hinzugefügt
Signed-off-by: jhenning <jhenning@students.uni-mainz.de>
</commit_message>
<xml_diff>
--- a/DMnetkit/Kantenverteilung.xlsx
+++ b/DMnetkit/Kantenverteilung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12435" tabRatio="873"/>
   </bookViews>
   <sheets>
     <sheet name="GESAMT" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="577">
   <si>
     <t>Anzahl Knoten</t>
   </si>
@@ -1753,6 +1753,21 @@
   <si>
     <t>Anzahl Klassen</t>
   </si>
+  <si>
+    <t>Durchmesser:</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Komplett zusammenhängend:</t>
+  </si>
+  <si>
+    <t>KomplettZusammenhängend:</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
 </sst>
 </file>
 
@@ -3635,11 +3650,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146806704"/>
-        <c:axId val="146807088"/>
+        <c:axId val="184518256"/>
+        <c:axId val="185065064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146806704"/>
+        <c:axId val="184518256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3682,7 +3697,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146807088"/>
+        <c:crossAx val="185065064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3690,7 +3705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146807088"/>
+        <c:axId val="185065064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3741,7 +3756,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146806704"/>
+        <c:crossAx val="184518256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -5266,11 +5281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147595968"/>
-        <c:axId val="147596360"/>
+        <c:axId val="183838720"/>
+        <c:axId val="185778312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147595968"/>
+        <c:axId val="183838720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5280,7 +5295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147596360"/>
+        <c:crossAx val="185778312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5288,7 +5303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147596360"/>
+        <c:axId val="185778312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5299,7 +5314,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147595968"/>
+        <c:crossAx val="183838720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8128,11 +8143,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147597144"/>
-        <c:axId val="147597536"/>
+        <c:axId val="185779488"/>
+        <c:axId val="186631456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147597144"/>
+        <c:axId val="185779488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8142,7 +8157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147597536"/>
+        <c:crossAx val="186631456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8150,7 +8165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147597536"/>
+        <c:axId val="186631456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8161,7 +8176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147597144"/>
+        <c:crossAx val="185779488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8926,11 +8941,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147598320"/>
-        <c:axId val="148139760"/>
+        <c:axId val="186632240"/>
+        <c:axId val="186632632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147598320"/>
+        <c:axId val="186632240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8940,7 +8955,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148139760"/>
+        <c:crossAx val="186632632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8948,7 +8963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148139760"/>
+        <c:axId val="186632632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8959,7 +8974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147598320"/>
+        <c:crossAx val="186632240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10166,11 +10181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146754776"/>
-        <c:axId val="146646464"/>
+        <c:axId val="184970696"/>
+        <c:axId val="184972104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146754776"/>
+        <c:axId val="184970696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10213,7 +10228,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146646464"/>
+        <c:crossAx val="184972104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10221,7 +10236,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146646464"/>
+        <c:axId val="184972104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10272,7 +10287,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146754776"/>
+        <c:crossAx val="184970696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14512,11 +14527,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146748328"/>
-        <c:axId val="147483216"/>
+        <c:axId val="184775208"/>
+        <c:axId val="184511904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146748328"/>
+        <c:axId val="184775208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14559,7 +14574,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147483216"/>
+        <c:crossAx val="184511904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14567,7 +14582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147483216"/>
+        <c:axId val="184511904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14618,7 +14633,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146748328"/>
+        <c:crossAx val="184775208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18498,11 +18513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147070560"/>
-        <c:axId val="147108152"/>
+        <c:axId val="185135928"/>
+        <c:axId val="185278056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147070560"/>
+        <c:axId val="185135928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18545,7 +18560,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147108152"/>
+        <c:crossAx val="185278056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18553,7 +18568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147108152"/>
+        <c:axId val="185278056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18604,7 +18619,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147070560"/>
+        <c:crossAx val="185135928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21004,11 +21019,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147189616"/>
-        <c:axId val="147194096"/>
+        <c:axId val="185027896"/>
+        <c:axId val="185183384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147189616"/>
+        <c:axId val="185027896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21018,7 +21033,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147194096"/>
+        <c:crossAx val="185183384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21026,7 +21041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147194096"/>
+        <c:axId val="185183384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21037,7 +21052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147189616"/>
+        <c:crossAx val="185027896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22666,11 +22681,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146030704"/>
-        <c:axId val="146031096"/>
+        <c:axId val="183839504"/>
+        <c:axId val="183839896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146030704"/>
+        <c:axId val="183839504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22680,7 +22695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146031096"/>
+        <c:crossAx val="183839896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22688,7 +22703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146031096"/>
+        <c:axId val="183839896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22699,7 +22714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146030704"/>
+        <c:crossAx val="183839504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25360,11 +25375,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146029920"/>
-        <c:axId val="146029528"/>
+        <c:axId val="183840680"/>
+        <c:axId val="183841072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146029920"/>
+        <c:axId val="183840680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25374,7 +25389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146029528"/>
+        <c:crossAx val="183841072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25382,7 +25397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146029528"/>
+        <c:axId val="183841072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25393,7 +25408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146029920"/>
+        <c:crossAx val="183840680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26362,11 +26377,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146030312"/>
-        <c:axId val="146028744"/>
+        <c:axId val="185775960"/>
+        <c:axId val="185776352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146030312"/>
+        <c:axId val="185775960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26376,7 +26391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146028744"/>
+        <c:crossAx val="185776352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26384,7 +26399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146028744"/>
+        <c:axId val="185776352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26395,7 +26410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146030312"/>
+        <c:crossAx val="185775960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -29908,11 +29923,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147594792"/>
-        <c:axId val="147595184"/>
+        <c:axId val="185777136"/>
+        <c:axId val="185777528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147594792"/>
+        <c:axId val="185777136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29922,7 +29937,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147595184"/>
+        <c:crossAx val="185777528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29930,7 +29945,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147595184"/>
+        <c:axId val="185777528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29941,7 +29956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147594792"/>
+        <c:crossAx val="185777136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -30648,9 +30663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177:B178"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30714,1005 +30731,1004 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>imdb_all!E74</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B7">
+        <f>imdb_all!F74</f>
+        <v>7</v>
+      </c>
+    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
+        <f>imdb_all!E75</f>
+        <v>Komplett zusammenhängend:</v>
+      </c>
+      <c r="B8" t="str">
+        <f>imdb_all!F75</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
         <f>imdb_all!E53</f>
         <v>AUC-NOTblockBuster-Final:</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B10" t="str">
         <f>imdb_all!F53</f>
         <v xml:space="preserve"> 0.8618437481513311 </v>
       </c>
-      <c r="C8" t="str">
+      <c r="C10" t="str">
         <f>imdb_all!G53</f>
         <v>(0.029342937073814922)</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
         <f>imdb_all!E54</f>
         <v>AUC-blockBuster-Final:</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B11" t="str">
         <f>imdb_all!F54</f>
         <v xml:space="preserve"> 0.8635299759223048 </v>
       </c>
-      <c r="C9" t="str">
+      <c r="C11" t="str">
         <f>imdb_all!G54</f>
         <v>(0.02805032838301136)</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
         <f>imdb_prodco!E40</f>
         <v>imdb_prodco</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <f>imdb_prodco!F40</f>
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <f>imdb_prodco!G40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>569</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <f>imdb_prodco!$E$2</f>
         <v>14.099236641221374</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
         <f>imdb_prodco!E58</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <f>imdb_prodco!F58</f>
         <v>1441</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <f>imdb_prodco!G58</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
         <f>imdb_prodco!E59</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <f>imdb_prodco!F59</f>
         <v>20317</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <f>imdb_prodco!G59</f>
         <v>40634</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
         <f>imdb_prodco!E60</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <f>imdb_prodco!F60</f>
         <v>2</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <f>imdb_prodco!G60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>imdb_prodco!E63</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B19">
+        <f>imdb_prodco!F63</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>imdb_prodco!E64</f>
+        <v>Komplett zusammenhängend:</v>
+      </c>
+      <c r="B20" t="str">
+        <f>imdb_prodco!F64</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
         <f>imdb_prodco!E41</f>
         <v xml:space="preserve">AUC-NOTblockBuster-Final: </v>
       </c>
-      <c r="B18" t="str">
+      <c r="B22" t="str">
         <f>imdb_prodco!F41</f>
         <v xml:space="preserve">0.8588265524219333 </v>
       </c>
-      <c r="C18" t="str">
+      <c r="C22" t="str">
         <f>imdb_prodco!G41</f>
         <v>(0.03616439486233569)</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <f>imdb_prodco!E42</f>
         <v xml:space="preserve">AUC-blockBuster-Final: </v>
       </c>
-      <c r="B19" t="str">
+      <c r="B23" t="str">
         <f>imdb_prodco!F42</f>
         <v xml:space="preserve">0.8563516018493212 </v>
       </c>
-      <c r="C19" t="str">
+      <c r="C23" t="str">
         <f>imdb_prodco!G42</f>
         <v>(0.037250584019606986)</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
         <f>cora_all!E61</f>
         <v>cora_all</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>569</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <f>cora_all!$E$2</f>
         <v>16.939622641509434</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
         <f>cora_all!E99</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B24">
+      <c r="B28">
         <f>cora_all!F99</f>
         <v>4240</v>
       </c>
-      <c r="C24">
+      <c r="C28">
         <f>cora_all!G99</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
         <f>cora_all!E100</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B25">
+      <c r="B29">
         <f>cora_all!F100</f>
         <v>71824</v>
       </c>
-      <c r="C25">
+      <c r="C29">
         <f>cora_all!G100</f>
         <v>71824</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
         <f>cora_all!E101</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B26">
+      <c r="B30">
         <f>cora_all!F101</f>
         <v>7</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <f>cora_all!G101</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>cora_all!E104</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B31">
+        <f>cora_all!F104</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>cora_all!E105</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B32" t="str">
+        <f>cora_all!F105</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
         <f>cora_all!E62</f>
         <v>AUC-RuleLearning-Final:</v>
       </c>
-      <c r="B28" t="str">
+      <c r="B34" t="str">
         <f>cora_all!F62</f>
         <v>0.9742898681596355</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C34" t="str">
         <f>cora_all!G62</f>
         <v>(0.022450725663630426)</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
         <f>cora_all!E63</f>
         <v>AUC-ReinforcementLearning-Final:</v>
       </c>
-      <c r="B29" t="str">
+      <c r="B35" t="str">
         <f>cora_all!F63</f>
         <v>0.9695840448109253</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C35" t="str">
         <f>cora_all!G63</f>
         <v>(0.015257600398157645)</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
         <f>cora_all!E64</f>
         <v>AUC-Theory-Final:</v>
       </c>
-      <c r="B30" t="str">
+      <c r="B36" t="str">
         <f>cora_all!F64</f>
         <v>0.953652154540249</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C36" t="str">
         <f>cora_all!G64</f>
         <v>(0.01610414858137884)</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
         <f>cora_all!E65</f>
         <v>AUC-NeuralNetworks-Final:</v>
       </c>
-      <c r="B31" t="str">
+      <c r="B37" t="str">
         <f>cora_all!F65</f>
         <v>0.9406137976533255</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C37" t="str">
         <f>cora_all!G65</f>
         <v>(0.013334547640091869)</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
         <f>cora_all!E66</f>
         <v>AUC-ProbabilisticMethods-Final:</v>
       </c>
-      <c r="B32" t="str">
+      <c r="B38" t="str">
         <f>cora_all!F66</f>
         <v>0.969349385856576</v>
       </c>
-      <c r="C32" t="str">
+      <c r="C38" t="str">
         <f>cora_all!G66</f>
         <v>(0.015206669608278305)</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
         <f>cora_all!E67</f>
         <v>AUC-GeneticAlgorithms-Final:</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B39" t="str">
         <f>cora_all!F67</f>
         <v>0.984516500196654</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C39" t="str">
         <f>cora_all!G67</f>
         <v>(0.007423123444253344)</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
         <f>cora_all!E68</f>
         <v>AUC-CaseBased-Final:</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B40" t="str">
         <f>cora_all!F68</f>
         <v>0.9675731117325865</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C40" t="str">
         <f>cora_all!G68</f>
         <v>(0.01553783564122287)</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="str">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
         <f>cora_cite!E74</f>
         <v>cora_cite</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>569</v>
       </c>
-      <c r="B38">
+      <c r="B44">
         <f>cora_cite!$E$1</f>
         <v>5.310377358490566</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
         <f>cora_cite!E112</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B39">
+      <c r="B45">
         <f>cora_cite!F112</f>
         <v>4240</v>
       </c>
-      <c r="C39">
+      <c r="C45">
         <f>cora_cite!G112</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
         <f>cora_cite!E113</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B40">
+      <c r="B46">
         <f>cora_cite!F113</f>
         <v>22516</v>
       </c>
-      <c r="C40">
+      <c r="C46">
         <f>cora_cite!G113</f>
         <v>22516</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
         <f>cora_cite!E114</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B41">
+      <c r="B47">
         <f>cora_cite!F114</f>
         <v>7</v>
       </c>
-      <c r="C41">
+      <c r="C47">
         <f>cora_cite!G114</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="str">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>cora_cite!E117</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B48">
+        <f>cora_cite!F117</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>cora_cite!E118</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B49" t="str">
+        <f>cora_cite!F118</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
         <f>cora_cite!E75</f>
         <v>AUC-RuleLearning-Final:</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B51" t="str">
         <f>cora_cite!F75</f>
         <v>0.9499319059209326</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C51" t="str">
         <f>cora_cite!G75</f>
         <v>(0.027458458047380237)</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
         <f>cora_cite!E76</f>
         <v>AUC-ReinforcementLearning-Final:</v>
       </c>
-      <c r="B44" t="str">
+      <c r="B52" t="str">
         <f>cora_cite!F76</f>
         <v>0.9594669064291873</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C52" t="str">
         <f>cora_cite!G76</f>
         <v>(0.031338793819323585)</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
         <f>cora_cite!E77</f>
         <v>AUC-Theory-Final:</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B53" t="str">
         <f>cora_cite!F77</f>
         <v>0.9346096301604943</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C53" t="str">
         <f>cora_cite!G77</f>
         <v>(0.016442670194944158)</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
         <f>cora_cite!E78</f>
         <v>AUC-NeuralNetworks-Final:</v>
       </c>
-      <c r="B46" t="str">
+      <c r="B54" t="str">
         <f>cora_cite!F78</f>
         <v>0.918904708886328</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C54" t="str">
         <f>cora_cite!G78</f>
         <v>(0.01483929154267815)</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
         <f>cora_cite!E79</f>
         <v>AUC-ProbabilisticMethods-Final:</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B55" t="str">
         <f>cora_cite!F79</f>
         <v>0.9446940577125366</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C55" t="str">
         <f>cora_cite!G79</f>
         <v>(0.013846988242017522)</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
         <f>cora_cite!E80</f>
         <v>AUC-GeneticAlgorithms-Final:</v>
       </c>
-      <c r="B48" t="str">
+      <c r="B56" t="str">
         <f>cora_cite!F80</f>
         <v>0.9808472781108545</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C56" t="str">
         <f>cora_cite!G80</f>
         <v>(0.0066739906108290396)</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
         <f>cora_cite!E81</f>
         <v>AUC-CaseBased-Final:</v>
       </c>
-      <c r="B49" t="str">
+      <c r="B57" t="str">
         <f>cora_cite!F81</f>
         <v>0.9484988160914737</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C57" t="str">
         <f>cora_cite!G81</f>
         <v>(0.015719955562677412)</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="str">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="str">
         <f>'WebKB-cornell-cocite'!E54</f>
         <v>webkb_cornell_cocite</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>569</v>
       </c>
-      <c r="B53">
+      <c r="B61">
         <f>'WebKB-cornell-cocite'!$E$2</f>
         <v>76.444444444444443</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
         <f>'WebKB-cornell-cocite'!E88</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B54">
+      <c r="B62">
         <f>'WebKB-cornell-cocite'!F88</f>
         <v>351</v>
       </c>
-      <c r="C54">
+      <c r="C62">
         <f>'WebKB-cornell-cocite'!G88</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
         <f>'WebKB-cornell-cocite'!E89</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B55">
+      <c r="B63">
         <f>'WebKB-cornell-cocite'!F89</f>
         <v>26832</v>
       </c>
-      <c r="C55">
+      <c r="C63">
         <f>'WebKB-cornell-cocite'!G89</f>
         <v>26832</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
         <f>'WebKB-cornell-cocite'!E90</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B56">
+      <c r="B64">
         <f>'WebKB-cornell-cocite'!F90</f>
         <v>6</v>
       </c>
-      <c r="C56">
+      <c r="C64">
         <f>'WebKB-cornell-cocite'!G90</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>'WebKB-cornell-cocite'!E93</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B65">
+        <f>'WebKB-cornell-cocite'!F93</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>'WebKB-cornell-cocite'!E94</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B66" t="str">
+        <f>'WebKB-cornell-cocite'!F94</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
         <f>'WebKB-cornell-cocite'!E55</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B58" t="str">
+      <c r="B68" t="str">
         <f>'WebKB-cornell-cocite'!F55</f>
         <v>0.8431556159232942</v>
       </c>
-      <c r="C58" t="str">
+      <c r="C68" t="str">
         <f>'WebKB-cornell-cocite'!G55</f>
         <v>(0.08352274359180378)</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
         <f>'WebKB-cornell-cocite'!E56</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B59" t="str">
+      <c r="B69" t="str">
         <f>'WebKB-cornell-cocite'!F56</f>
         <v>0.8246793659621803</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C69" t="str">
         <f>'WebKB-cornell-cocite'!G56</f>
         <v>(0.1604453592074772)</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
         <f>'WebKB-cornell-cocite'!E57</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B60" t="str">
+      <c r="B70" t="str">
         <f>'WebKB-cornell-cocite'!F57</f>
         <v>0.8589135065925684</v>
       </c>
-      <c r="C60" t="str">
+      <c r="C70" t="str">
         <f>'WebKB-cornell-cocite'!G57</f>
         <v>(0.05920075912453466)</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
         <f>'WebKB-cornell-cocite'!E58</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B61" t="str">
+      <c r="B71" t="str">
         <f>'WebKB-cornell-cocite'!F58</f>
         <v>0.7502862048786886</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C71" t="str">
         <f>'WebKB-cornell-cocite'!G58</f>
         <v>(0.09389817878529888)</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="str">
         <f>'WebKB-cornell-cocite'!E59</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B62" t="str">
+      <c r="B72" t="str">
         <f>'WebKB-cornell-cocite'!F59</f>
         <v>0.7260018903455809</v>
       </c>
-      <c r="C62" t="str">
+      <c r="C72" t="str">
         <f>'WebKB-cornell-cocite'!G59</f>
         <v>(0.3041605558302911)</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="str">
         <f>'WebKB-cornell-cocite'!E60</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B63" t="str">
+      <c r="B73" t="str">
         <f>'WebKB-cornell-cocite'!F60</f>
         <v>0.38467023172905523</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C73" t="str">
         <f>'WebKB-cornell-cocite'!G60</f>
         <v>(0.4328232653900865)</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="str">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="str">
         <f>'WebKB-cornell-link1'!E57</f>
         <v>webkb_cornell_link1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>569</v>
       </c>
-      <c r="B67">
+      <c r="B77">
         <f>'WebKB-cornell-link1'!$E$2</f>
         <v>3.9686609686609686</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="str">
         <f>'WebKB-cornell-link1'!E91</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B68">
+      <c r="B78">
         <f>'WebKB-cornell-link1'!F91</f>
         <v>351</v>
       </c>
-      <c r="C68">
+      <c r="C78">
         <f>'WebKB-cornell-link1'!G91</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
         <f>'WebKB-cornell-link1'!E92</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B69">
+      <c r="B79">
         <f>'WebKB-cornell-link1'!F92</f>
         <v>1393</v>
       </c>
-      <c r="C69">
+      <c r="C79">
         <f>'WebKB-cornell-link1'!G92</f>
         <v>1393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="str">
         <f>'WebKB-cornell-link1'!E93</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B70">
+      <c r="B80">
         <f>'WebKB-cornell-link1'!F93</f>
         <v>6</v>
       </c>
-      <c r="C70">
+      <c r="C80">
         <f>'WebKB-cornell-link1'!G93</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
+        <f>'WebKB-cornell-link1'!E96</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B81">
+        <f>'WebKB-cornell-link1'!F96</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f>'WebKB-cornell-link1'!E97</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B82" t="str">
+        <f>'WebKB-cornell-link1'!F97</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
         <f>'WebKB-cornell-link1'!E58</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B72" t="str">
+      <c r="B84" t="str">
         <f>'WebKB-cornell-link1'!F58</f>
         <v>0.6912272407998215</v>
       </c>
-      <c r="C72" t="str">
+      <c r="C84" t="str">
         <f>'WebKB-cornell-link1'!G58</f>
         <v>(0.12043841233415016)</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="str">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
         <f>'WebKB-cornell-link1'!E59</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B73" t="str">
+      <c r="B85" t="str">
         <f>'WebKB-cornell-link1'!F59</f>
         <v>0.8139315845621263</v>
       </c>
-      <c r="C73" t="str">
+      <c r="C85" t="str">
         <f>'WebKB-cornell-link1'!G59</f>
         <v>(0.10669616809029236)</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
         <f>'WebKB-cornell-link1'!E60</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B74" t="str">
+      <c r="B86" t="str">
         <f>'WebKB-cornell-link1'!F60</f>
         <v>0.474418990630369</v>
       </c>
-      <c r="C74" t="str">
+      <c r="C86" t="str">
         <f>'WebKB-cornell-link1'!G60</f>
         <v>(0.14215031966672612)</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
         <f>'WebKB-cornell-link1'!E61</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B75" t="str">
+      <c r="B87" t="str">
         <f>'WebKB-cornell-link1'!F61</f>
         <v>0.6236096986125769</v>
       </c>
-      <c r="C75" t="str">
+      <c r="C87" t="str">
         <f>'WebKB-cornell-link1'!G61</f>
         <v>(0.11538605242499193)</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="str">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
         <f>'WebKB-cornell-link1'!E62</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B76" t="str">
+      <c r="B88" t="str">
         <f>'WebKB-cornell-link1'!F62</f>
         <v>0.6637604723707666</v>
       </c>
-      <c r="C76" t="str">
+      <c r="C88" t="str">
         <f>'WebKB-cornell-link1'!G62</f>
         <v>(0.15445667658526022)</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="str">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
         <f>'WebKB-cornell-link1'!E63</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B77" t="str">
+      <c r="B89" t="str">
         <f>'WebKB-cornell-link1'!F63</f>
         <v>0.25588235294117645</v>
       </c>
-      <c r="C77" t="str">
+      <c r="C89" t="str">
         <f>'WebKB-cornell-link1'!G63</f>
         <v>(0.27029324642302716)</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="str">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="str">
         <f>'WebKB-texas-cocite'!E61</f>
         <v>webkb_texas_cocite</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>569</v>
       </c>
-      <c r="B81">
+      <c r="B93">
         <f>'WebKB-texas-cocite'!$E$2</f>
         <v>97.597633136094672</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="str">
         <f>'WebKB-texas-cocite'!E95</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B82">
+      <c r="B94">
         <f>'WebKB-texas-cocite'!F95</f>
         <v>338</v>
       </c>
-      <c r="C82">
+      <c r="C94">
         <f>'WebKB-texas-cocite'!G95</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="str">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
         <f>'WebKB-texas-cocite'!E96</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B83">
+      <c r="B95">
         <f>'WebKB-texas-cocite'!F96</f>
         <v>32988</v>
       </c>
-      <c r="C83">
+      <c r="C95">
         <f>'WebKB-texas-cocite'!G96</f>
         <v>32988</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="str">
         <f>'WebKB-texas-cocite'!E97</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B84">
+      <c r="B96">
         <f>'WebKB-texas-cocite'!F97</f>
         <v>6</v>
       </c>
-      <c r="C84">
+      <c r="C96">
         <f>'WebKB-texas-cocite'!G97</f>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="str">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="str">
+        <f>'WebKB-texas-cocite'!E100</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B97">
+        <f>'WebKB-texas-cocite'!F100</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>'WebKB-texas-cocite'!E101</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B98" t="str">
+        <f>'WebKB-texas-cocite'!F101</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
         <f>'WebKB-texas-cocite'!E62</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B86" t="str">
+      <c r="B100" t="str">
         <f>'WebKB-texas-cocite'!F62</f>
         <v>0.941360894453567</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C100" t="str">
         <f>'WebKB-texas-cocite'!G62</f>
         <v>(0.06455821277131375)</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="str">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="str">
         <f>'WebKB-texas-cocite'!E63</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B87" t="str">
+      <c r="B101" t="str">
         <f>'WebKB-texas-cocite'!F63</f>
         <v>0.9285362263184844</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C101" t="str">
         <f>'WebKB-texas-cocite'!G63</f>
         <v>(0.05479184088042997)</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="str">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
         <f>'WebKB-texas-cocite'!E64</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B88" t="str">
+      <c r="B102" t="str">
         <f>'WebKB-texas-cocite'!F64</f>
         <v>0.9355753393858233</v>
       </c>
-      <c r="C88" t="str">
+      <c r="C102" t="str">
         <f>'WebKB-texas-cocite'!G64</f>
         <v>(0.06920397069572812)</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="str">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="str">
         <f>'WebKB-texas-cocite'!E65</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B89" t="str">
+      <c r="B103" t="str">
         <f>'WebKB-texas-cocite'!F65</f>
         <v>0.966565017799538</v>
       </c>
-      <c r="C89" t="str">
+      <c r="C103" t="str">
         <f>'WebKB-texas-cocite'!G65</f>
         <v>(0.027895778730252663)</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="str">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="str">
         <f>'WebKB-texas-cocite'!E66</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B90" t="str">
+      <c r="B104" t="str">
         <f>'WebKB-texas-cocite'!F66</f>
         <v>0.8902406796459216</v>
       </c>
-      <c r="C90" t="str">
+      <c r="C104" t="str">
         <f>'WebKB-texas-cocite'!G66</f>
         <v>(0.0839555807372096)</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="str">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="str">
         <f>'WebKB-texas-cocite'!E67</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B91" t="str">
+      <c r="B105" t="str">
         <f>'WebKB-texas-cocite'!F67</f>
         <v>0.2570869990224829</v>
       </c>
-      <c r="C91" t="str">
+      <c r="C105" t="str">
         <f>'WebKB-texas-cocite'!G67</f>
         <v>(0.3952581955707154)</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="str">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="str">
         <f>'WebKB-texas-link1'!E54</f>
         <v>webkb_texas_link1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>569</v>
-      </c>
-      <c r="B95">
-        <f>'WebKB-texas-link1'!$E$2</f>
-        <v>2.9644970414201182</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="str">
-        <f>'WebKB-texas-link1'!E88</f>
-        <v>Anzahl Knoten</v>
-      </c>
-      <c r="B96">
-        <f>'WebKB-texas-link1'!F88</f>
-        <v>338</v>
-      </c>
-      <c r="C96">
-        <f>'WebKB-texas-link1'!G88</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="str">
-        <f>'WebKB-texas-link1'!E89</f>
-        <v>Anzahl Kanten</v>
-      </c>
-      <c r="B97">
-        <f>'WebKB-texas-link1'!F89</f>
-        <v>1002</v>
-      </c>
-      <c r="C97">
-        <f>'WebKB-texas-link1'!G89</f>
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="str">
-        <f>'WebKB-texas-link1'!E90</f>
-        <v>Anzahl Klassen</v>
-      </c>
-      <c r="B98">
-        <f>'WebKB-texas-link1'!F90</f>
-        <v>6</v>
-      </c>
-      <c r="C98">
-        <f>'WebKB-texas-link1'!G90</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="str">
-        <f>'WebKB-texas-link1'!E55</f>
-        <v>AUC-faculty-Final:</v>
-      </c>
-      <c r="B100" t="str">
-        <f>'WebKB-texas-link1'!F55</f>
-        <v>0.5078936128835322</v>
-      </c>
-      <c r="C100" t="str">
-        <f>'WebKB-texas-link1'!G55</f>
-        <v>(0.11357698195325452)</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="str">
-        <f>'WebKB-texas-link1'!E56</f>
-        <v>AUC-course-Final:</v>
-      </c>
-      <c r="B101" t="str">
-        <f>'WebKB-texas-link1'!F56</f>
-        <v>0.4798993410803756</v>
-      </c>
-      <c r="C101" t="str">
-        <f>'WebKB-texas-link1'!G56</f>
-        <v>(0.1478423680476221)</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="str">
-        <f>'WebKB-texas-link1'!E57</f>
-        <v>AUC-department-Final:</v>
-      </c>
-      <c r="B102" t="str">
-        <f>'WebKB-texas-link1'!F57</f>
-        <v>0.7227153246271711</v>
-      </c>
-      <c r="C102" t="str">
-        <f>'WebKB-texas-link1'!G57</f>
-        <v>(0.17996261626478655)</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="str">
-        <f>'WebKB-texas-link1'!E58</f>
-        <v>AUC-student-Final:</v>
-      </c>
-      <c r="B103" t="str">
-        <f>'WebKB-texas-link1'!F58</f>
-        <v>0.40563593946675347</v>
-      </c>
-      <c r="C103" t="str">
-        <f>'WebKB-texas-link1'!G58</f>
-        <v>(0.06673174711771074)</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="str">
-        <f>'WebKB-texas-link1'!E59</f>
-        <v>AUC-project-Final:</v>
-      </c>
-      <c r="B104" t="str">
-        <f>'WebKB-texas-link1'!F59</f>
-        <v>0.5222320184604667</v>
-      </c>
-      <c r="C104" t="str">
-        <f>'WebKB-texas-link1'!G59</f>
-        <v>(0.1843544903103284)</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="str">
-        <f>'WebKB-texas-link1'!E60</f>
-        <v>AUC-staff-Final:</v>
-      </c>
-      <c r="B105" t="str">
-        <f>'WebKB-texas-link1'!F60</f>
-        <v>0.25</v>
-      </c>
-      <c r="C105" t="str">
-        <f>'WebKB-texas-link1'!G60</f>
-        <v>(0.41013397389537226)</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="str">
-        <f>'WebKB-washington-cocite'!E59</f>
-        <v>webkb_washington_cocite</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -31720,555 +31736,792 @@
         <v>569</v>
       </c>
       <c r="B109">
+        <f>'WebKB-texas-link1'!$E$2</f>
+        <v>2.9644970414201182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="str">
+        <f>'WebKB-texas-link1'!E88</f>
+        <v>Anzahl Knoten</v>
+      </c>
+      <c r="B110">
+        <f>'WebKB-texas-link1'!F88</f>
+        <v>338</v>
+      </c>
+      <c r="C110">
+        <f>'WebKB-texas-link1'!G88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="str">
+        <f>'WebKB-texas-link1'!E89</f>
+        <v>Anzahl Kanten</v>
+      </c>
+      <c r="B111">
+        <f>'WebKB-texas-link1'!F89</f>
+        <v>1002</v>
+      </c>
+      <c r="C111">
+        <f>'WebKB-texas-link1'!G89</f>
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="str">
+        <f>'WebKB-texas-link1'!E90</f>
+        <v>Anzahl Klassen</v>
+      </c>
+      <c r="B112">
+        <f>'WebKB-texas-link1'!F90</f>
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <f>'WebKB-texas-link1'!G90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="str">
+        <f>'WebKB-texas-link1'!E93</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B113">
+        <f>'WebKB-texas-link1'!F93</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="str">
+        <f>'WebKB-texas-link1'!E94</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B114" t="str">
+        <f>'WebKB-texas-link1'!F94</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="str">
+        <f>'WebKB-texas-link1'!E55</f>
+        <v>AUC-faculty-Final:</v>
+      </c>
+      <c r="B116" t="str">
+        <f>'WebKB-texas-link1'!F55</f>
+        <v>0.5078936128835322</v>
+      </c>
+      <c r="C116" t="str">
+        <f>'WebKB-texas-link1'!G55</f>
+        <v>(0.11357698195325452)</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
+        <f>'WebKB-texas-link1'!E56</f>
+        <v>AUC-course-Final:</v>
+      </c>
+      <c r="B117" t="str">
+        <f>'WebKB-texas-link1'!F56</f>
+        <v>0.4798993410803756</v>
+      </c>
+      <c r="C117" t="str">
+        <f>'WebKB-texas-link1'!G56</f>
+        <v>(0.1478423680476221)</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="str">
+        <f>'WebKB-texas-link1'!E57</f>
+        <v>AUC-department-Final:</v>
+      </c>
+      <c r="B118" t="str">
+        <f>'WebKB-texas-link1'!F57</f>
+        <v>0.7227153246271711</v>
+      </c>
+      <c r="C118" t="str">
+        <f>'WebKB-texas-link1'!G57</f>
+        <v>(0.17996261626478655)</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f>'WebKB-texas-link1'!E58</f>
+        <v>AUC-student-Final:</v>
+      </c>
+      <c r="B119" t="str">
+        <f>'WebKB-texas-link1'!F58</f>
+        <v>0.40563593946675347</v>
+      </c>
+      <c r="C119" t="str">
+        <f>'WebKB-texas-link1'!G58</f>
+        <v>(0.06673174711771074)</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="str">
+        <f>'WebKB-texas-link1'!E59</f>
+        <v>AUC-project-Final:</v>
+      </c>
+      <c r="B120" t="str">
+        <f>'WebKB-texas-link1'!F59</f>
+        <v>0.5222320184604667</v>
+      </c>
+      <c r="C120" t="str">
+        <f>'WebKB-texas-link1'!G59</f>
+        <v>(0.1843544903103284)</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="str">
+        <f>'WebKB-texas-link1'!E60</f>
+        <v>AUC-staff-Final:</v>
+      </c>
+      <c r="B121" t="str">
+        <f>'WebKB-texas-link1'!F60</f>
+        <v>0.25</v>
+      </c>
+      <c r="C121" t="str">
+        <f>'WebKB-texas-link1'!G60</f>
+        <v>(0.41013397389537226)</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="str">
+        <f>'WebKB-washington-cocite'!E59</f>
+        <v>webkb_washington_cocite</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>569</v>
+      </c>
+      <c r="B125">
         <f>30462/434</f>
         <v>70.188940092165893</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="str">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="str">
         <f>'WebKB-washington-cocite'!E93</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B110">
+      <c r="B126">
         <f>'WebKB-washington-cocite'!F93</f>
         <v>434</v>
       </c>
-      <c r="C110">
+      <c r="C126">
         <f>'WebKB-washington-cocite'!G93</f>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="str">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="str">
         <f>'WebKB-washington-cocite'!E94</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B111">
+      <c r="B127">
         <f>'WebKB-washington-cocite'!F94</f>
         <v>30462</v>
       </c>
-      <c r="C111">
+      <c r="C127">
         <f>'WebKB-washington-cocite'!G94</f>
         <v>30462</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="str">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="str">
         <f>'WebKB-washington-cocite'!E95</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B112">
+      <c r="B128">
         <f>'WebKB-washington-cocite'!F95</f>
         <v>6</v>
       </c>
-      <c r="C112">
+      <c r="C128">
         <f>'WebKB-washington-cocite'!G95</f>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="str">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="str">
+        <f>'WebKB-washington-cocite'!E98</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B129">
+        <f>'WebKB-washington-cocite'!F98</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="str">
+        <f>'WebKB-washington-cocite'!E99</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B130" t="str">
+        <f>'WebKB-washington-cocite'!F99</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="str">
         <f>'WebKB-washington-cocite'!E60</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B114" t="str">
+      <c r="B132" t="str">
         <f>'WebKB-washington-cocite'!F60</f>
         <v>0.9050879592055423</v>
       </c>
-      <c r="C114" t="str">
+      <c r="C132" t="str">
         <f>'WebKB-washington-cocite'!G60</f>
         <v>(0.04374592971201586)</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="str">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="str">
         <f>'WebKB-washington-cocite'!E61</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B115" t="str">
+      <c r="B133" t="str">
         <f>'WebKB-washington-cocite'!F61</f>
         <v>0.9422411144487397</v>
       </c>
-      <c r="C115" t="str">
+      <c r="C133" t="str">
         <f>'WebKB-washington-cocite'!G61</f>
         <v>(0.037751380004413804)</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="str">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="str">
         <f>'WebKB-washington-cocite'!E62</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B116" t="str">
+      <c r="B134" t="str">
         <f>'WebKB-washington-cocite'!F62</f>
         <v>0.7189294745873693</v>
       </c>
-      <c r="C116" t="str">
+      <c r="C134" t="str">
         <f>'WebKB-washington-cocite'!G62</f>
         <v>(0.22536364833114653)</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="str">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
         <f>'WebKB-washington-cocite'!E63</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B117" t="str">
+      <c r="B135" t="str">
         <f>'WebKB-washington-cocite'!F63</f>
         <v>0.8152837726628126</v>
       </c>
-      <c r="C117" t="str">
+      <c r="C135" t="str">
         <f>'WebKB-washington-cocite'!G63</f>
         <v>(0.07010325225732056)</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="str">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
         <f>'WebKB-washington-cocite'!E64</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B118" t="str">
+      <c r="B136" t="str">
         <f>'WebKB-washington-cocite'!F64</f>
         <v>0.6610742867219753</v>
       </c>
-      <c r="C118" t="str">
+      <c r="C136" t="str">
         <f>'WebKB-washington-cocite'!G64</f>
         <v>(0.2920614360170532)</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="str">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="str">
         <f>'WebKB-washington-cocite'!E65</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B119" t="str">
+      <c r="B137" t="str">
         <f>'WebKB-washington-cocite'!F65</f>
         <v>0.483484798430913</v>
       </c>
-      <c r="C119" t="str">
+      <c r="C137" t="str">
         <f>'WebKB-washington-cocite'!G65</f>
         <v>(0.42991040366746436)</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="str">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="str">
         <f>'WebKB-washington-link1'!E62</f>
         <v>webkb_washington_link1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>569</v>
       </c>
-      <c r="B123">
+      <c r="B141">
         <f>'WebKB-washington-link1'!$E$2</f>
         <v>4.4723502304147464</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="str">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
         <f>'WebKB-washington-link1'!E96</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B124">
+      <c r="B142">
         <f>'WebKB-washington-link1'!F96</f>
         <v>434</v>
       </c>
-      <c r="C124">
+      <c r="C142">
         <f>'WebKB-washington-link1'!G96</f>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="str">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
         <f>'WebKB-washington-link1'!E97</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B125">
+      <c r="B143">
         <f>'WebKB-washington-link1'!F97</f>
         <v>1941</v>
       </c>
-      <c r="C125">
+      <c r="C143">
         <f>'WebKB-washington-link1'!G97</f>
         <v>1941</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="str">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="str">
         <f>'WebKB-washington-link1'!E98</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B126">
+      <c r="B144">
         <f>'WebKB-washington-link1'!F98</f>
         <v>6</v>
       </c>
-      <c r="C126">
+      <c r="C144">
         <f>'WebKB-washington-link1'!G98</f>
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="str">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="str">
+        <f>'WebKB-washington-link1'!E101</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B145">
+        <f>'WebKB-washington-link1'!F101</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="str">
+        <f>'WebKB-washington-link1'!E102</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B146" t="str">
+        <f>'WebKB-washington-link1'!F102</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="str">
         <f>'WebKB-washington-link1'!E63</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B128" t="str">
+      <c r="B148" t="str">
         <f>'WebKB-washington-link1'!F63</f>
         <v>0.5821586041727358</v>
       </c>
-      <c r="C128" t="str">
+      <c r="C148" t="str">
         <f>'WebKB-washington-link1'!G63</f>
         <v>(0.09996950961244942)</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="str">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="str">
         <f>'WebKB-washington-link1'!E64</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B129" t="str">
+      <c r="B149" t="str">
         <f>'WebKB-washington-link1'!F64</f>
         <v>0.8646045615791509</v>
       </c>
-      <c r="C129" t="str">
+      <c r="C149" t="str">
         <f>'WebKB-washington-link1'!G64</f>
         <v>(0.05969266727040029)</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="str">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="str">
         <f>'WebKB-washington-link1'!E65</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B130" t="str">
+      <c r="B150" t="str">
         <f>'WebKB-washington-link1'!F65</f>
         <v>0.6541350635618126</v>
       </c>
-      <c r="C130" t="str">
+      <c r="C150" t="str">
         <f>'WebKB-washington-link1'!G65</f>
         <v>(0.1389585863724436)</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="str">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="str">
         <f>'WebKB-washington-link1'!E66</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B131" t="str">
+      <c r="B151" t="str">
         <f>'WebKB-washington-link1'!F66</f>
         <v>0.724192822422925</v>
       </c>
-      <c r="C131" t="str">
+      <c r="C151" t="str">
         <f>'WebKB-washington-link1'!G66</f>
         <v>(0.10124889561964975)</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="str">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="str">
         <f>'WebKB-washington-link1'!E67</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B132" t="str">
+      <c r="B152" t="str">
         <f>'WebKB-washington-link1'!F67</f>
         <v>0.5453691399040237</v>
       </c>
-      <c r="C132" t="str">
+      <c r="C152" t="str">
         <f>'WebKB-washington-link1'!G67</f>
         <v>(0.22972291591031344)</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="str">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="str">
         <f>'WebKB-washington-link1'!E68</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B133" t="str">
+      <c r="B153" t="str">
         <f>'WebKB-washington-link1'!F68</f>
         <v>0.39027293844367017</v>
       </c>
-      <c r="C133" t="str">
+      <c r="C153" t="str">
         <f>'WebKB-washington-link1'!G68</f>
         <v>(0.3619720582676422)</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="str">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="str">
         <f>'WebKB-wisconsin-cocite'!E50</f>
         <v>webkb_wisconsin_cocite</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>569</v>
       </c>
-      <c r="B137">
+      <c r="B157">
         <f>'WebKB-wisconsin-cocite'!$E$2</f>
         <v>93.951977401129938</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="str">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="str">
         <f>'WebKB-wisconsin-cocite'!E84</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B138">
+      <c r="B158">
         <f>'WebKB-wisconsin-cocite'!F84</f>
         <v>354</v>
       </c>
-      <c r="C138">
+      <c r="C158">
         <f>'WebKB-wisconsin-cocite'!G84</f>
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="str">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="str">
         <f>'WebKB-wisconsin-cocite'!E85</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B139">
+      <c r="B159">
         <f>'WebKB-wisconsin-cocite'!F85</f>
         <v>33250</v>
       </c>
-      <c r="C139">
+      <c r="C159">
         <f>'WebKB-wisconsin-cocite'!G85</f>
         <v>33250</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="str">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="str">
         <f>'WebKB-wisconsin-cocite'!E86</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B140">
+      <c r="B160">
         <f>'WebKB-wisconsin-cocite'!F86</f>
         <v>6</v>
       </c>
-      <c r="C140">
+      <c r="C160">
         <f>'WebKB-wisconsin-cocite'!G86</f>
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="str">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="str">
+        <f>'WebKB-wisconsin-cocite'!E89</f>
+        <v>Durchmesser:</v>
+      </c>
+      <c r="B161">
+        <f>'WebKB-wisconsin-cocite'!F89</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="str">
+        <f>'WebKB-wisconsin-cocite'!E90</f>
+        <v>KomplettZusammenhängend:</v>
+      </c>
+      <c r="B162" t="str">
+        <f>'WebKB-wisconsin-cocite'!F90</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="str">
         <f>'WebKB-wisconsin-cocite'!E51</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B142" t="str">
+      <c r="B164" t="str">
         <f>'WebKB-wisconsin-cocite'!F51</f>
         <v>0.9676042663476874</v>
       </c>
-      <c r="C142" t="str">
+      <c r="C164" t="str">
         <f>'WebKB-wisconsin-cocite'!G51</f>
         <v>(0.037519211998940406)</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="str">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="str">
         <f>'WebKB-wisconsin-cocite'!E52</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B143" t="str">
+      <c r="B165" t="str">
         <f>'WebKB-wisconsin-cocite'!F52</f>
         <v>0.9725941938668647</v>
       </c>
-      <c r="C143" t="str">
+      <c r="C165" t="str">
         <f>'WebKB-wisconsin-cocite'!G52</f>
         <v>(0.029268795472602062)</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="str">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="str">
         <f>'WebKB-wisconsin-cocite'!E53</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B144" t="str">
+      <c r="B166" t="str">
         <f>'WebKB-wisconsin-cocite'!F53</f>
         <v>0.6151272910557184</v>
       </c>
-      <c r="C144" t="str">
+      <c r="C166" t="str">
         <f>'WebKB-wisconsin-cocite'!G53</f>
         <v>(0.2445906998082489)</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="str">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="str">
         <f>'WebKB-wisconsin-cocite'!E54</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B145" t="str">
+      <c r="B167" t="str">
         <f>'WebKB-wisconsin-cocite'!F54</f>
         <v>0.9016696399478658</v>
       </c>
-      <c r="C145" t="str">
+      <c r="C167" t="str">
         <f>'WebKB-wisconsin-cocite'!G54</f>
         <v>(0.12131990150139868)</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="str">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="str">
         <f>'WebKB-wisconsin-cocite'!E55</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B146" t="str">
+      <c r="B168" t="str">
         <f>'WebKB-wisconsin-cocite'!F55</f>
         <v>0.9748137788839877</v>
       </c>
-      <c r="C146" t="str">
+      <c r="C168" t="str">
         <f>'WebKB-wisconsin-cocite'!G55</f>
         <v>(0.020597837561693512)</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="str">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="str">
         <f>'WebKB-wisconsin-cocite'!E56</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B147" t="str">
+      <c r="B169" t="str">
         <f>'WebKB-wisconsin-cocite'!F56</f>
         <v>0.7354176215940922</v>
       </c>
-      <c r="C147" t="str">
+      <c r="C169" t="str">
         <f>'WebKB-wisconsin-cocite'!G56</f>
         <v>(0.39173331818826035)</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="str">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="str">
         <f>'WebKB-wisconsin-link1'!E57</f>
         <v>webkb_wisconsin_link1</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>569</v>
       </c>
-      <c r="B151">
+      <c r="B173">
         <f>'WebKB-wisconsin-link1'!$E$2</f>
         <v>3.2627118644067798</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="str">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="str">
         <f>'WebKB-wisconsin-link1'!E91</f>
         <v>Anzahl Knoten</v>
       </c>
-      <c r="B152">
+      <c r="B174">
         <f>'WebKB-wisconsin-link1'!F91</f>
         <v>354</v>
       </c>
-      <c r="C152">
+      <c r="C174">
         <f>'WebKB-wisconsin-link1'!G91</f>
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="str">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="str">
         <f>'WebKB-wisconsin-link1'!E92</f>
         <v>Anzahl Kanten</v>
       </c>
-      <c r="B153">
+      <c r="B175">
         <f>'WebKB-wisconsin-link1'!F92</f>
         <v>1155</v>
       </c>
-      <c r="C153">
+      <c r="C175">
         <f>'WebKB-wisconsin-link1'!G92</f>
         <v>1155</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="str">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="str">
         <f>'WebKB-wisconsin-link1'!E93</f>
         <v>Anzahl Klassen</v>
       </c>
-      <c r="B154">
+      <c r="B176">
         <f>'WebKB-wisconsin-link1'!F93</f>
         <v>6</v>
       </c>
-      <c r="C154">
+      <c r="C176">
         <f>'WebKB-wisconsin-link1'!G93</f>
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="str">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>572</v>
+      </c>
+      <c r="B177">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>575</v>
+      </c>
+      <c r="B178" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="str">
         <f>'WebKB-wisconsin-link1'!E58</f>
         <v>AUC-student-Final:</v>
       </c>
-      <c r="B156" t="str">
+      <c r="B180" t="str">
         <f>'WebKB-wisconsin-link1'!F58</f>
         <v>0.3729811843038651</v>
       </c>
-      <c r="C156" t="str">
+      <c r="C180" t="str">
         <f>'WebKB-wisconsin-link1'!G58</f>
         <v>(0.09902256520851029)</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="str">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="str">
         <f>'WebKB-wisconsin-link1'!E59</f>
         <v>AUC-course-Final:</v>
       </c>
-      <c r="B157" t="str">
+      <c r="B181" t="str">
         <f>'WebKB-wisconsin-link1'!F59</f>
         <v>0.6126281213004556</v>
       </c>
-      <c r="C157" t="str">
+      <c r="C181" t="str">
         <f>'WebKB-wisconsin-link1'!G59</f>
         <v>(0.08822940709261416)</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="str">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="str">
         <f>'WebKB-wisconsin-link1'!E60</f>
         <v>AUC-faculty-Final:</v>
       </c>
-      <c r="B158" t="str">
+      <c r="B182" t="str">
         <f>'WebKB-wisconsin-link1'!F60</f>
         <v>0.417271534469115</v>
       </c>
-      <c r="C158" t="str">
+      <c r="C182" t="str">
         <f>'WebKB-wisconsin-link1'!G60</f>
         <v>(0.1111066947623341)</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="str">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="str">
         <f>'WebKB-wisconsin-link1'!E61</f>
         <v>AUC-department-Final:</v>
       </c>
-      <c r="B159" t="str">
+      <c r="B183" t="str">
         <f>'WebKB-wisconsin-link1'!F61</f>
         <v>0.8274751208319756</v>
       </c>
-      <c r="C159" t="str">
+      <c r="C183" t="str">
         <f>'WebKB-wisconsin-link1'!G61</f>
         <v>(0.11991677512017498)</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="str">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="str">
         <f>'WebKB-wisconsin-link1'!E62</f>
         <v>AUC-project-Final:</v>
       </c>
-      <c r="B160" t="str">
+      <c r="B184" t="str">
         <f>'WebKB-wisconsin-link1'!F62</f>
         <v>0.5548772007235495</v>
       </c>
-      <c r="C160" t="str">
+      <c r="C184" t="str">
         <f>'WebKB-wisconsin-link1'!G62</f>
         <v>(0.34059082968291404)</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="str">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="str">
         <f>'WebKB-wisconsin-link1'!E63</f>
         <v>AUC-staff-Final:</v>
       </c>
-      <c r="B161" t="str">
+      <c r="B185" t="str">
         <f>'WebKB-wisconsin-link1'!F63</f>
         <v>0.48070409982174683</v>
       </c>
-      <c r="C161" t="str">
+      <c r="C185" t="str">
         <f>'WebKB-wisconsin-link1'!G63</f>
         <v>(0.37500882164276567)</v>
       </c>
@@ -32282,8 +32535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G575"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="E85" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33317,7 +33570,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>1</v>
       </c>
@@ -33325,23 +33578,35 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>572</v>
+      </c>
+      <c r="F98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99">
         <v>96</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>575</v>
+      </c>
+      <c r="F99" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0</v>
       </c>
@@ -33349,7 +33614,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>1</v>
       </c>
@@ -33357,7 +33622,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0</v>
       </c>
@@ -33365,7 +33630,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0</v>
       </c>
@@ -33373,7 +33638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>0</v>
       </c>
@@ -33381,7 +33646,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>1</v>
       </c>
@@ -33389,7 +33654,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>0</v>
       </c>
@@ -33397,7 +33662,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>0</v>
       </c>
@@ -33405,7 +33670,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>0</v>
       </c>
@@ -33413,7 +33678,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>2</v>
       </c>
@@ -33421,7 +33686,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0</v>
       </c>
@@ -33429,7 +33694,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>0</v>
       </c>
@@ -33437,7 +33702,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>0</v>
       </c>
@@ -37159,8 +37424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G239"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="E94" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101:F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38234,6 +38499,12 @@
       <c r="C101">
         <v>98</v>
       </c>
+      <c r="E101" t="s">
+        <v>572</v>
+      </c>
+      <c r="F101">
+        <v>9</v>
+      </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102">
@@ -38241,6 +38512,12 @@
       </c>
       <c r="C102">
         <v>99</v>
+      </c>
+      <c r="E102" t="s">
+        <v>575</v>
+      </c>
+      <c r="F102" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
@@ -39349,8 +39626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G461"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D89" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89:F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40327,6 +40604,12 @@
       <c r="C89">
         <v>86</v>
       </c>
+      <c r="E89" t="s">
+        <v>572</v>
+      </c>
+      <c r="F89">
+        <v>4</v>
+      </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90">
@@ -40334,6 +40617,12 @@
       </c>
       <c r="C90">
         <v>87</v>
+      </c>
+      <c r="E90" t="s">
+        <v>575</v>
+      </c>
+      <c r="F90" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -43314,8 +43603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G117"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96:F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44349,16 +44638,28 @@
       <c r="C96">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>572</v>
+      </c>
+      <c r="F96">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>575</v>
+      </c>
+      <c r="F97" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0</v>
       </c>
@@ -44366,7 +44667,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0</v>
       </c>
@@ -44374,7 +44675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0</v>
       </c>
@@ -44382,7 +44683,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0</v>
       </c>
@@ -44390,7 +44691,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0</v>
       </c>
@@ -44398,7 +44699,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0</v>
       </c>
@@ -44406,7 +44707,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>0</v>
       </c>
@@ -44414,7 +44715,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>0</v>
       </c>
@@ -44422,7 +44723,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>0</v>
       </c>
@@ -44430,7 +44731,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>0</v>
       </c>
@@ -44438,7 +44739,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>0</v>
       </c>
@@ -44446,7 +44747,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>0</v>
       </c>
@@ -44454,7 +44755,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0</v>
       </c>
@@ -44462,7 +44763,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>0</v>
       </c>
@@ -44470,7 +44771,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>0</v>
       </c>
@@ -44528,8 +44829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G289"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F75" sqref="E74:F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45239,6 +45540,12 @@
       <c r="C74">
         <v>71</v>
       </c>
+      <c r="E74" t="s">
+        <v>572</v>
+      </c>
+      <c r="F74">
+        <v>7</v>
+      </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75">
@@ -45246,6 +45553,12 @@
       </c>
       <c r="C75">
         <v>72</v>
+      </c>
+      <c r="E75" t="s">
+        <v>574</v>
+      </c>
+      <c r="F75" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
@@ -46971,8 +47284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G184"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F64" sqref="E63:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47595,6 +47908,12 @@
       <c r="C63">
         <v>60</v>
       </c>
+      <c r="E63" t="s">
+        <v>572</v>
+      </c>
+      <c r="F63">
+        <v>9</v>
+      </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64">
@@ -47602,6 +47921,12 @@
       </c>
       <c r="C64">
         <v>61</v>
+      </c>
+      <c r="E64" t="s">
+        <v>574</v>
+      </c>
+      <c r="F64" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -48574,8 +48899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G685"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104:F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49708,6 +50033,12 @@
       <c r="C104">
         <v>101</v>
       </c>
+      <c r="E104" t="s">
+        <v>572</v>
+      </c>
+      <c r="F104">
+        <v>11</v>
+      </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105">
@@ -49715,6 +50046,12 @@
       </c>
       <c r="C105">
         <v>102</v>
+      </c>
+      <c r="E105" t="s">
+        <v>575</v>
+      </c>
+      <c r="F105" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
@@ -54367,8 +54704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G625"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55605,6 +55942,12 @@
       <c r="C117">
         <v>114</v>
       </c>
+      <c r="E117" t="s">
+        <v>572</v>
+      </c>
+      <c r="F117">
+        <v>16</v>
+      </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118">
@@ -55612,6 +55955,12 @@
       </c>
       <c r="C118">
         <v>115</v>
+      </c>
+      <c r="E118" t="s">
+        <v>575</v>
+      </c>
+      <c r="F118" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
@@ -59680,8 +60029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G385"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="E82" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93:F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60690,6 +61039,12 @@
       <c r="C93">
         <v>90</v>
       </c>
+      <c r="E93" t="s">
+        <v>572</v>
+      </c>
+      <c r="F93">
+        <v>4</v>
+      </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94">
@@ -60697,6 +61052,12 @@
       </c>
       <c r="C94">
         <v>91</v>
+      </c>
+      <c r="E94" t="s">
+        <v>575</v>
+      </c>
+      <c r="F94" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
@@ -63037,8 +63398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G261"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D82" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96:F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64071,16 +64432,28 @@
       <c r="C96">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>572</v>
+      </c>
+      <c r="F96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>575</v>
+      </c>
+      <c r="F97" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0</v>
       </c>
@@ -64088,7 +64461,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0</v>
       </c>
@@ -64096,7 +64469,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0</v>
       </c>
@@ -64104,7 +64477,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0</v>
       </c>
@@ -64112,7 +64485,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0</v>
       </c>
@@ -64120,7 +64493,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0</v>
       </c>
@@ -64128,7 +64501,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>0</v>
       </c>
@@ -64136,7 +64509,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>0</v>
       </c>
@@ -64144,7 +64517,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>0</v>
       </c>
@@ -64152,7 +64525,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>0</v>
       </c>
@@ -64160,7 +64533,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>0</v>
       </c>
@@ -64168,7 +64541,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>0</v>
       </c>
@@ -64176,7 +64549,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0</v>
       </c>
@@ -64184,7 +64557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>0</v>
       </c>
@@ -64192,7 +64565,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>0</v>
       </c>
@@ -65402,8 +65775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G433"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D97" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66468,6 +66841,12 @@
       <c r="C100">
         <v>97</v>
       </c>
+      <c r="E100" t="s">
+        <v>572</v>
+      </c>
+      <c r="F100">
+        <v>5</v>
+      </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101">
@@ -66475,6 +66854,12 @@
       </c>
       <c r="C101">
         <v>98</v>
+      </c>
+      <c r="E101" t="s">
+        <v>575</v>
+      </c>
+      <c r="F101" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -69143,8 +69528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G151"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="E88" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70153,6 +70538,12 @@
       <c r="C93">
         <v>90</v>
       </c>
+      <c r="E93" t="s">
+        <v>572</v>
+      </c>
+      <c r="F93">
+        <v>10</v>
+      </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94">
@@ -70160,6 +70551,12 @@
       </c>
       <c r="C94">
         <v>91</v>
+      </c>
+      <c r="E94" t="s">
+        <v>575</v>
+      </c>
+      <c r="F94" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>